<commit_message>
make compatible with demultiplexing
</commit_message>
<xml_diff>
--- a/tests/simulate/structure.xlsx
+++ b/tests/simulate/structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gary/Downloads/zivi/data/counts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gary/Downloads/zivi/git/delt-core/tests/simulate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1E46FA-724E-3C4D-BB27-5A2806BEE480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14787123-FD33-6542-B287-CB6B7A1A2873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,6 +80,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,6 +95,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,11 +133,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -438,9 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -465,7 +468,7 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0</v>
       </c>
       <c r="D2">
@@ -479,7 +482,7 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0</v>
       </c>
       <c r="D3">
@@ -493,7 +496,7 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0</v>
       </c>
       <c r="D4">
@@ -507,7 +510,7 @@
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0</v>
       </c>
       <c r="D5">
@@ -521,7 +524,7 @@
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0</v>
       </c>
       <c r="D6">
@@ -535,7 +538,7 @@
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>0</v>
       </c>
       <c r="D7">
@@ -549,7 +552,7 @@
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>0</v>
       </c>
       <c r="D8">

</xml_diff>